<commit_message>
updated codes and deleted "no effect" line in DAG 19
</commit_message>
<xml_diff>
--- a/terms_mapped_to_codes.xlsx
+++ b/terms_mapped_to_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\Master Project\wise-dag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48DF16A-D2BE-406A-9C2C-08F42712FAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F8D5F6-F508-476A-AD81-0EE93143ADB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1724EB86-F306-47F4-ABEC-FB51705565F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1724EB86-F306-47F4-ABEC-FB51705565F8}"/>
   </bookViews>
   <sheets>
     <sheet name="terms" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="320">
   <si>
     <t>Diabetes</t>
   </si>
@@ -952,31 +952,34 @@
     <t>time</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>88003-9</t>
-  </si>
-  <si>
     <t>direction</t>
   </si>
   <si>
     <t>switch</t>
   </si>
   <si>
-    <t>Endothelial microvesicles?</t>
-  </si>
-  <si>
-    <t>Leukocyte-derived microvesicles?</t>
-  </si>
-  <si>
     <t>concept_code_2</t>
   </si>
   <si>
     <t>term</t>
   </si>
   <si>
-    <t>dysbalance code</t>
+    <t>Endothelial microvesicles</t>
+  </si>
+  <si>
+    <t>Leukocyte-derived microvesicles</t>
+  </si>
+  <si>
+    <t>Non-atherosclerotic abnormalities</t>
+  </si>
+  <si>
+    <t>Reactive Oxygen Species production</t>
+  </si>
+  <si>
+    <t>Cardiac remodeling</t>
+  </si>
+  <si>
+    <t>Loss of brain structural integrity</t>
   </si>
 </sst>
 </file>
@@ -1839,14 +1842,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D181B-FC1A-461E-92A1-3F55E3525786}">
   <dimension ref="A1:E309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A298" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F306" sqref="F306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="67.9296875" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.59765625" customWidth="1"/>
     <col min="3" max="3" width="21.46484375" customWidth="1"/>
     <col min="4" max="4" width="9.9296875" customWidth="1"/>
     <col min="5" max="5" width="15.796875" customWidth="1"/>
@@ -1854,19 +1857,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B1" t="s">
         <v>308</v>
       </c>
       <c r="C1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D1" t="s">
         <v>309</v>
       </c>
       <c r="E1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -2005,8 +2008,8 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>311</v>
+      <c r="B17">
+        <v>422504002</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -2434,7 +2437,7 @@
         <v>373930000</v>
       </c>
       <c r="E66" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.45">
@@ -2468,8 +2471,8 @@
       <c r="B70">
         <v>72308001</v>
       </c>
-      <c r="C70" t="s">
-        <v>318</v>
+      <c r="C70">
+        <v>263654008</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
@@ -2638,8 +2641,11 @@
       <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89" t="s">
-        <v>310</v>
+      <c r="B89">
+        <v>246300000</v>
+      </c>
+      <c r="C89">
+        <v>72167002</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.45">
@@ -2832,7 +2838,7 @@
         <v>248153007</v>
       </c>
       <c r="E112" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -3139,7 +3145,7 @@
         <v>248153007</v>
       </c>
       <c r="E150" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.45">
@@ -3162,8 +3168,11 @@
       <c r="A153" t="s">
         <v>151</v>
       </c>
-      <c r="B153" t="s">
-        <v>310</v>
+      <c r="B153">
+        <v>246300000</v>
+      </c>
+      <c r="C153">
+        <v>40146001</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.45">
@@ -3229,8 +3238,8 @@
       <c r="A161" t="s">
         <v>159</v>
       </c>
-      <c r="B161" t="s">
-        <v>310</v>
+      <c r="B161">
+        <v>74937006</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.45">
@@ -3337,7 +3346,7 @@
         <v>248153007</v>
       </c>
       <c r="E174" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.45">
@@ -3465,7 +3474,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.45">
@@ -3484,7 +3493,7 @@
         <v>1325171000000100</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>191</v>
       </c>
@@ -3492,7 +3501,7 @@
         <v>31653004</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>192</v>
       </c>
@@ -3500,7 +3509,7 @@
         <v>31996006</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>193</v>
       </c>
@@ -3508,15 +3517,18 @@
         <v>69116000</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>194</v>
       </c>
-      <c r="B196" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B196">
+        <v>417357006</v>
+      </c>
+      <c r="C196">
+        <v>39823006</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>195</v>
       </c>
@@ -3524,15 +3536,15 @@
         <v>422504002</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>197</v>
       </c>
@@ -3540,7 +3552,7 @@
         <v>365782006</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>198</v>
       </c>
@@ -3548,7 +3560,7 @@
         <v>38716007</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>199</v>
       </c>
@@ -3556,7 +3568,7 @@
         <v>71395006</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>200</v>
       </c>
@@ -3564,7 +3576,7 @@
         <v>13644009</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>201</v>
       </c>
@@ -3572,7 +3584,7 @@
         <v>414086009</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>202</v>
       </c>
@@ -3580,7 +3592,7 @@
         <v>439127006</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>203</v>
       </c>
@@ -3588,7 +3600,7 @@
         <v>230698000</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>204</v>
       </c>
@@ -3596,7 +3608,7 @@
         <v>49436004</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>205</v>
       </c>
@@ -3604,7 +3616,7 @@
         <v>248153007</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>206</v>
       </c>
@@ -3625,7 +3637,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.45">
@@ -3668,7 +3680,7 @@
         <v>256235009</v>
       </c>
       <c r="E215" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.45">
@@ -3965,7 +3977,7 @@
         <v>248153007</v>
       </c>
       <c r="E248" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.45">
@@ -4408,7 +4420,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.45">
@@ -4479,7 +4491,7 @@
         <v>405152002</v>
       </c>
       <c r="E304" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
fixed excel rounding long numbers and postprocess term list, export terms together with concept names to csv
</commit_message>
<xml_diff>
--- a/terms_mapped_to_codes.xlsx
+++ b/terms_mapped_to_codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\Master Project\wise-dag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F8D5F6-F508-476A-AD81-0EE93143ADB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704D673D-AAB4-4940-9FBB-79D1C087C985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1724EB86-F306-47F4-ABEC-FB51705565F8}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="322">
   <si>
     <t>Diabetes</t>
   </si>
@@ -980,6 +980,12 @@
   </si>
   <si>
     <t>Loss of brain structural integrity</t>
+  </si>
+  <si>
+    <t>726499301000119105</t>
+  </si>
+  <si>
+    <t>16837681000119104</t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1469,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1842,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D181B-FC1A-461E-92A1-3F55E3525786}">
   <dimension ref="A1:E309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F306" sqref="F306"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2590,16 +2597,16 @@
       <c r="A83" t="s">
         <v>81</v>
       </c>
-      <c r="B83">
-        <v>7.2649930100011904E+17</v>
+      <c r="B83" s="1" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>82</v>
       </c>
-      <c r="B84">
-        <v>1.68376810001191E+16</v>
+      <c r="B84" s="1" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.45">
@@ -3490,7 +3497,7 @@
         <v>190</v>
       </c>
       <c r="B192">
-        <v>1325171000000100</v>
+        <v>840539006</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>